<commit_message>
Database entity model completed
</commit_message>
<xml_diff>
--- a/Docs/DBModel.xlsx
+++ b/Docs/DBModel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\Net Banking Project\NetBanking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2808D76F-F063-42C2-B208-19AD4B776AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E54F5F8-2ACD-4BDA-8474-509A985A67B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2325" yWindow="-13890" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>